<commit_message>
update task a2; add task a3;
</commit_message>
<xml_diff>
--- a/hexp1989/evidence.xlsx
+++ b/hexp1989/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26700" windowHeight="13340" activeTab="2"/>
+    <workbookView windowWidth="26700" windowHeight="13340" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="39">
   <si>
     <t>TeamName</t>
   </si>
@@ -97,10 +97,31 @@
     <t>A1249C880C55A25774317E957B21F25E4E0571312CB3E574C5D54ED4534F4524</t>
   </si>
   <si>
-    <t>9EBEA09D8F0A2D89D44B428CDF29358FF6878F91A69919A580BD86A468458F1C</t>
+    <t>hexp1989m</t>
+  </si>
+  <si>
+    <t>395BEC57E7571C2CB100769A962A872105BA147FEC006B591D5DB56338286725</t>
+  </si>
+  <si>
+    <t>hexp198901</t>
+  </si>
+  <si>
+    <t>8CE3162EE0F4F54BAC7117C0C58084B40A590651D55765E93869535073551200</t>
+  </si>
+  <si>
+    <t>hexp198902</t>
   </si>
   <si>
     <t>ChainID</t>
+  </si>
+  <si>
+    <t>15426D1062AF12E42BB5A2AD63D0B76EED099C02B40EFCBD81816BF0B4E5C852</t>
+  </si>
+  <si>
+    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/ark/hexp1989</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
   </si>
   <si>
     <t>tx hash on irisnet</t>
@@ -2257,10 +2278,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2360,10 +2381,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2463,10 +2484,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2566,10 +2587,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2661,7 +2682,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -2669,10 +2690,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2680,7 +2701,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -2689,7 +2710,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -2768,7 +2789,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -2776,10 +2797,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2787,7 +2808,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -2796,7 +2817,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -2875,7 +2896,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -2883,10 +2904,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2894,7 +2915,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -2903,7 +2924,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -2982,7 +3003,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -2990,10 +3011,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3001,7 +3022,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3010,7 +3031,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3089,7 +3110,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -3097,10 +3118,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3108,7 +3129,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3117,7 +3138,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3196,7 +3217,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -3204,10 +3225,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3215,7 +3236,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3224,7 +3245,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3405,7 +3426,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -3413,10 +3434,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3424,7 +3445,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3433,7 +3454,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3512,7 +3533,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -3520,10 +3541,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3531,7 +3552,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3540,7 +3561,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3624,7 +3645,7 @@
     </row>
     <row r="2" ht="16.4" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3633,7 +3654,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3724,7 +3745,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3733,7 +3754,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3824,7 +3845,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3833,7 +3854,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3924,7 +3945,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3933,7 +3954,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -4003,8 +4024,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4035,28 +4056,34 @@
         <v>16</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
@@ -4116,13 +4143,14 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="2" width="17.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.8515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6171875" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.8515625" style="1" customWidth="1"/>
@@ -4139,22 +4167,22 @@
         <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E2" s="4"/>
     </row>
@@ -4251,22 +4279,22 @@
         <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E2" s="4"/>
     </row>
@@ -4363,22 +4391,22 @@
         <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E2" s="4"/>
     </row>
@@ -4476,22 +4504,22 @@
         <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E2" s="4"/>
     </row>
@@ -4589,10 +4617,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -4692,10 +4720,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>

</xml_diff>

<commit_message>
fix stage 1 evidence
</commit_message>
<xml_diff>
--- a/hexp1989/evidence.xlsx
+++ b/hexp1989/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26700" windowHeight="13340" activeTab="6"/>
+    <workbookView windowWidth="26700" windowHeight="13260" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
   <si>
     <t>TeamName</t>
   </si>
@@ -73,7 +73,13 @@
     <t>stars1aw0jfqlg4ulhnleytpydvmx0zem33828usn5nt</t>
   </si>
   <si>
+    <t>juno1aw0jfqlg4ulhnleytpydvmx0zem33828778jlx</t>
+  </si>
+  <si>
     <t>uptick1ft9rkjpqa9pyygyw5cp2wjwxu6cn2gjzp0dv3s</t>
+  </si>
+  <si>
+    <t>omniflix1aw0jfqlg4ulhnleytpydvmx0zem338284j4s0y</t>
   </si>
   <si>
     <t>MartyMou#4999</t>
@@ -97,58 +103,43 @@
     <t>NFTID</t>
   </si>
   <si>
-    <t>C8532A50073E612015107CA3A441B4EDE239E71DE211783515836834EF3BC0A8</t>
+    <t>F02DF866606388ABDF5A9197D29AA89C4AA6744ADF7C5F2184CE7022DEEEDCE4</t>
   </si>
   <si>
-    <t>firstnft</t>
+    <t>nft1</t>
   </si>
   <si>
-    <t>4A584891081AC7675E78EC147FD8A2F05B2AE99D16ED50F07EF50A0C4FEB4E35</t>
+    <t>2DDBF3CFE56AFBB2CC994AE09D2D393D76C670B6ED5AD067B68334E73674EA6E</t>
   </si>
   <si>
-    <t>secondnft</t>
-  </si>
-  <si>
-    <t>CEA83C33CC4EC660F213810E440F851EB54B1A90026FC2A91B93955AA229A94B</t>
-  </si>
-  <si>
-    <t>thirdnft</t>
+    <t>nft2</t>
   </si>
   <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>4417522CDF5848A96BD94390D226623481C6079BC9BC3B661DAF0534C365E9C3</t>
+    <t>FE758DB82E969C2CB91F80718EA3766001C5B8532915FCA044C4BEF7FCD5D743</t>
   </si>
   <si>
-    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/arkhexp1989</t>
+    <t>stars15gth2r2nuhlmuwly2vqys4cd895aep6sc082e0fnxklzg5y44resndfwze</t>
   </si>
   <si>
     <t>elgafar-1</t>
   </si>
   <si>
-    <t>566FBB3A461DDCD09BB53F8D6D85A2FAC1B1F473E8E08277CBC4939186D9282A</t>
+    <t>3C699E949F9EDB4852CA1399152621C0520E314555374B86AC8C485C727077F9</t>
   </si>
   <si>
-    <t>nft-transfer/channel-3/arkhexp1989</t>
+    <t>ibc/E82E152600DC84D0FF8343DAFDAF8CBA532AD5775DC1039E5BD0D01952EED1DB</t>
   </si>
   <si>
     <t>uptick_7000-2</t>
   </si>
   <si>
-    <t>87B4271B5696C60D834DFB2E9252FF2E6DD1F91A7FF1BF9529084C65C095DE92</t>
+    <t>2F8059856936A3BF218911278A3DDAFCE18F4CF4DA3CAFBBFEC0C309F58615DB</t>
   </si>
   <si>
-    <t>stars15gth2r2nuhlmuwly2vqys4cd895aep6sc082e0fnxklzg5y44resndfwze</t>
-  </si>
-  <si>
-    <t>gon-irishub-1</t>
-  </si>
-  <si>
-    <t>A0DB06A16E66F8CB8563F1A042DB4E257C4D54164E51C294A2E46BE082ADFEA7</t>
-  </si>
-  <si>
-    <t>ibc/E82E152600DC84D0FF8343DAFDAF8CBA532AD5775DC1039E5BD0D01952EED1DB</t>
+    <t>5F4338B3B1A029EB71570C3BDFC63264737C90C84200298D30EF7984F5075E46</t>
   </si>
   <si>
     <t>ibc class on chain</t>
@@ -177,10 +168,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -204,22 +195,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,9 +231,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,8 +286,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,30 +304,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,6 +318,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
@@ -318,30 +332,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,61 +359,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,7 +401,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,13 +455,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,19 +497,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,61 +521,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -650,7 +641,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -659,7 +650,33 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -675,21 +692,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -723,159 +725,148 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2105,7 +2096,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="7"/>
@@ -2157,16 +2148,20 @@
       <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="G2" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:8">
@@ -2276,10 +2271,10 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -2287,10 +2282,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2379,10 +2374,10 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -2390,10 +2385,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2482,10 +2477,10 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -2493,10 +2488,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2585,10 +2580,10 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -2596,10 +2591,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2688,7 +2683,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>25</v>
@@ -2699,10 +2694,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2710,7 +2705,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -2719,7 +2714,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -2795,7 +2790,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>25</v>
@@ -2806,10 +2801,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2817,7 +2812,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -2826,7 +2821,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -2902,7 +2897,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>25</v>
@@ -2913,10 +2908,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2924,7 +2919,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -2933,7 +2928,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3009,7 +3004,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>25</v>
@@ -3020,10 +3015,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3031,7 +3026,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3040,7 +3035,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3116,7 +3111,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>25</v>
@@ -3127,10 +3122,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3138,7 +3133,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3147,7 +3142,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3223,7 +3218,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>25</v>
@@ -3234,10 +3229,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3245,7 +3240,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3254,7 +3249,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3318,7 +3313,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -3329,10 +3324,10 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -3340,10 +3335,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3432,7 +3427,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>25</v>
@@ -3443,10 +3438,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3454,7 +3449,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3463,7 +3458,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3539,7 +3534,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>25</v>
@@ -3550,10 +3545,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3561,7 +3556,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3570,7 +3565,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3645,7 +3640,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -3654,7 +3649,7 @@
     </row>
     <row r="2" ht="16.4" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3663,7 +3658,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3745,7 +3740,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -3754,7 +3749,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3763,7 +3758,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3845,7 +3840,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -3854,7 +3849,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3863,7 +3858,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3945,7 +3940,7 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -3954,7 +3949,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3963,7 +3958,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -4034,7 +4029,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4046,53 +4041,47 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="A4" s="7"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
@@ -4153,7 +4142,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4167,13 +4156,13 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>25</v>
@@ -4188,7 +4177,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>28</v>
@@ -4266,7 +4255,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4279,13 +4268,13 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>25</v>
@@ -4300,7 +4289,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>31</v>
@@ -4377,8 +4366,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4391,13 +4380,13 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>25</v>
@@ -4409,13 +4398,13 @@
         <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E2" s="4"/>
     </row>
@@ -4489,8 +4478,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4504,13 +4493,13 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>25</v>
@@ -4519,16 +4508,16 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" s="4"/>
     </row>
@@ -4615,10 +4604,10 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -4626,10 +4615,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -4718,10 +4707,10 @@
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -4729,10 +4718,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>

</xml_diff>

<commit_message>
stage 2. add A7-A9 tasks
</commit_message>
<xml_diff>
--- a/hexp1989/evidence.xlsx
+++ b/hexp1989/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26700" windowHeight="13260" activeTab="5"/>
+    <workbookView windowWidth="26700" windowHeight="13260" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="47">
   <si>
     <t>TeamName</t>
   </si>
@@ -140,6 +140,24 @@
   </si>
   <si>
     <t>5F4338B3B1A029EB71570C3BDFC63264737C90C84200298D30EF7984F5075E46</t>
+  </si>
+  <si>
+    <t>ibc/A79C1E10D480696A03D9DE4CFD1CF8E46E20B81186A15CF995D1DD5757E4A320</t>
+  </si>
+  <si>
+    <t>s2nft1</t>
+  </si>
+  <si>
+    <t>ibc/7BE58C51356817988DB2EC7BFD6C0B8F2B2DF32842DCDDC6AC160BFA4DBE1133</t>
+  </si>
+  <si>
+    <t>s2nft2</t>
+  </si>
+  <si>
+    <t>ibc/D34F1C115E1B24177F186BEE4B61538A424924AA524C4484F918D0DDA6D379DA</t>
+  </si>
+  <si>
+    <t>s2nft3</t>
   </si>
   <si>
     <t>ibc class on chain</t>
@@ -2095,8 +2113,8 @@
   <sheetPr/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="7"/>
@@ -2258,8 +2276,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -2282,10 +2300,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2362,7 +2380,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -2385,10 +2403,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2488,10 +2506,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2591,10 +2609,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2694,10 +2712,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2705,7 +2723,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -2714,7 +2732,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -2801,10 +2819,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2812,7 +2830,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -2821,7 +2839,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -2908,10 +2926,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2919,7 +2937,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -2928,7 +2946,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3015,10 +3033,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3026,7 +3044,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3035,7 +3053,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3122,10 +3140,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3133,7 +3151,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3142,7 +3160,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3229,10 +3247,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3240,7 +3258,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3249,7 +3267,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3438,10 +3456,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3449,7 +3467,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3458,7 +3476,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3545,10 +3563,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3556,7 +3574,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
@@ -3565,7 +3583,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
@@ -3649,7 +3667,7 @@
     </row>
     <row r="2" ht="16.4" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3658,7 +3676,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3749,7 +3767,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3758,7 +3776,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3849,7 +3867,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3858,7 +3876,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3949,7 +3967,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3958,7 +3976,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -4142,7 +4160,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4366,8 +4384,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4479,7 +4497,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4592,7 +4610,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4695,7 +4713,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -4718,10 +4736,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>

</xml_diff>

<commit_message>
Completed Stage 2 tasks
</commit_message>
<xml_diff>
--- a/hexp1989/evidence.xlsx
+++ b/hexp1989/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26700" windowHeight="13260" activeTab="9"/>
+    <workbookView windowWidth="26700" windowHeight="13260" firstSheet="11" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="87">
   <si>
     <t>TeamName</t>
   </si>
@@ -160,19 +160,139 @@
     <t>s2nft3</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
+    <t>ibc/EB5172D0C127327767A72960463C5EBB06F512C253DE40D2C19855EBDFE7D5DE</t>
+  </si>
+  <si>
+    <t>s2nft7</t>
+  </si>
+  <si>
+    <t>ibc/DF3C073D82E832969D3B9E7E8893BC642FFA52149DF9C9E8739F30FB0E0A05F0</t>
+  </si>
+  <si>
+    <t>s2nft8</t>
+  </si>
+  <si>
+    <t>ibc/84180FD2726F9DC296E749DBAB15351D7A07118A227C78BDD0DB26C56213F048</t>
+  </si>
+  <si>
+    <t>s2nft9</t>
+  </si>
+  <si>
+    <t>C66397329A2BFF57B9270056B88D1F2A3762030AA0A8BC80AB416EA9F1DA5638</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>28FAB3376F89C3013F7D8D666B0CB782AE4726E3FB1DDEEDCD9A766F2A40FAF2</t>
+  </si>
+  <si>
+    <t>468B6E1B50C374420527A5544FE94F01AB00C090246E23738AFCA0749A790401</t>
+  </si>
+  <si>
+    <t>81351F3FAF02F4A3E92219834D71673AB161FAA0ACD2F45535836EA915991455</t>
+  </si>
+  <si>
+    <t>9536A80261727D16E89D7EC45B3ABB75E351E4E031EB946C68C4F083F78892A8</t>
+  </si>
+  <si>
+    <t>E8566E1F9C3B2F0C8FB4BBA436D2C83F00E9470B122B0E189A271E9019D8C99B</t>
+  </si>
+  <si>
+    <t>8B6521DA0F40B75FD5B12F69D6F43DE1BBB44C5146580BBCAEEB92EE9A3FAEA9</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>05061FC93B0AEE029BA406DB2136F1099AADBEA52BB7D54100D903E70E8AAA96</t>
+  </si>
+  <si>
+    <t>6B47AE67A97FF717D58D11308FC5A09A468B7FEC68D0436D8CA0F2DCF9CB949A</t>
+  </si>
+  <si>
+    <t>DC245EDA5676F31D2F6BE7BD51235D44FDD1D507DA41C9C2B3F216EF26B9D8CE</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>FEDE9C7F24EEBED1EA4A420C9193E30FACC4024126F458966B2B61DB77E5C6D5</t>
+  </si>
+  <si>
+    <t>483B3E8007C3D72FF61EB84BDD2EB4F76111B05D3424070F4314268750F29047</t>
+  </si>
+  <si>
+    <t>F294C0D61729D73F0DA496D5D0F40E37D783ECB5D2DC474AC2B75F4273C344A5</t>
+  </si>
+  <si>
+    <t>5F9285893174BF675CD96EEB6CCF19D241FC8FC21E5BB95D8D9E95F7C93B5236</t>
+  </si>
+  <si>
+    <t>C992B3AB1D1579BA6F3E3CB13C4B397C0B57650CCFDF256D5FA5836C9B28FC20</t>
+  </si>
+  <si>
+    <t>260EF39ED1EEACD839240C5709EA61F4E33128AB009DBFCAB82FCF9574DF503F</t>
+  </si>
+  <si>
+    <t>2D517E8EC2F98723E135991A106F97F74E086A5500D8EB377DA9D006056D73C3</t>
+  </si>
+  <si>
+    <t>4422F2B6E62694F1F306B058BF32C9D27D9DFC4FCC34478FDD4A4801DA8B4C8F</t>
+  </si>
+  <si>
+    <t>D10D2B93A8E2F3F3850447C1B969AA2314E2E6EAF1C28B5FDBFFFF8F85B8D22F</t>
+  </si>
+  <si>
+    <t>ADBA25584023ECF595A2A726D8C0484C56BF23659EF7F7735A6696D2A61B9F11</t>
+  </si>
+  <si>
+    <t>A46341B56D1120FBA8682A565F682B2530E30B333EF4AB012F314037862A4289</t>
+  </si>
+  <si>
+    <t>5F069A1A8C05FCB7895A8B805AB2376F528E0B0A3346016B58990DBC24CC8DEE</t>
+  </si>
+  <si>
+    <t>D4F6F9E211BDFC08F809AA5F26CD209D0ED21E9AF621787B0AB96F65E687DA8F</t>
+  </si>
+  <si>
+    <t>7858890D58CEF24F7E1F6C6FDAB36F7AE8A75D8890D688FDBAE5E94933E92CBC</t>
+  </si>
+  <si>
+    <t>760AA208730A4C376AFAE521382E6F1C94F7AE56BEF12EC35C42D9EE8E3B8F70</t>
+  </si>
+  <si>
+    <t>95DA5AFC0BE92501BFC37CE2EB626F2E27D3F1095D385F10F60ED42A80D777B0</t>
+  </si>
+  <si>
+    <t>30873F75664D92A31F55ADC2D01E4E6E87B54DCAF6156F1BA5F22E1BF52A12F9</t>
+  </si>
+  <si>
+    <t>1C68DE4184251353C199C8E03FE6446FAADCCB8670B5A21C7507B3C78311FF55</t>
+  </si>
+  <si>
+    <t>27D471C98935E467709051850E9421DDF4BBDA5A3E538D8AFE0D31D5BF768694</t>
+  </si>
+  <si>
+    <t>61C6A277258C90DE71023CFED0EEBB9C81F3287CF7D7DD4220B21A5ADCE355C4</t>
+  </si>
+  <si>
+    <t>9791F4B360C166F2B8C3EE72DC6258A96F32A1C24FFCFB5621BA147CDF8357BD</t>
+  </si>
+  <si>
+    <t>82627167012075DC2B247EA0CA62E88E6247DA3AEA3BB3B0FEB64677EFA1A0FD</t>
+  </si>
+  <si>
+    <t>8BA774CD354BCFC510983BD4B17886534B72553D2D1EA95DC13D42DAB64CBC79</t>
+  </si>
+  <si>
+    <t>1F5134B751A27DB42E2AE3DE68E1A77BFA2B60AA46694EA796302F7EA329BDE3</t>
+  </si>
+  <si>
+    <t>2F57CE014C05D211661BA58FFDBEB400E9879EB6CF0AEAA9765045F6AF52ED63</t>
+  </si>
+  <si>
+    <t>71A741DCA096D666CE8F6AB5892213A5CDA6FC0AB6C50538AB90E9FBA4851924</t>
   </si>
   <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
@@ -186,10 +306,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -206,13 +326,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
@@ -226,11 +339,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -257,17 +370,60 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -276,21 +432,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -306,46 +447,25 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -377,7 +497,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,7 +509,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,85 +653,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,73 +677,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -646,11 +766,82 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -672,222 +863,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2276,7 +2396,7 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -2380,7 +2500,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -2483,7 +2603,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -2506,10 +2626,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2586,7 +2706,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -2609,10 +2729,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2689,7 +2809,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -2712,10 +2832,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2723,25 +2843,33 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>49</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -2796,7 +2924,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -2819,10 +2947,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2830,25 +2958,33 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>53</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -2903,7 +3039,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -2926,10 +3062,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2937,25 +3073,33 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>57</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -3010,7 +3154,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -3033,10 +3177,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3044,25 +3188,33 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>63</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -3117,7 +3269,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -3140,10 +3292,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3151,25 +3303,33 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -3224,7 +3384,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -3247,10 +3407,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3258,25 +3418,33 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -3432,8 +3600,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showGridLines="0" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -3456,10 +3624,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3467,39 +3635,55 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -3539,8 +3723,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -3563,10 +3747,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -3574,39 +3758,55 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>80</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -3667,7 +3867,7 @@
     </row>
     <row r="2" ht="16.4" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3676,7 +3876,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3767,7 +3967,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3776,7 +3976,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3867,7 +4067,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3876,7 +4076,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -3967,7 +4167,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3976,7 +4176,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>

</xml_diff>

<commit_message>
Add Stage 3. Completed B1 B2 tasks
</commit_message>
<xml_diff>
--- a/hexp1989/evidence.xlsx
+++ b/hexp1989/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26700" windowHeight="13260" firstSheet="11" activeTab="20"/>
+    <workbookView windowWidth="26700" windowHeight="13260" firstSheet="12" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t>TeamName</t>
   </si>
@@ -293,6 +293,18 @@
   </si>
   <si>
     <t>71A741DCA096D666CE8F6AB5892213A5CDA6FC0AB6C50538AB90E9FBA4851924</t>
+  </si>
+  <si>
+    <t>583FF646E8B2F03F233502845843D86DEBB2DA7647F32BC2903F813DDC179B36</t>
+  </si>
+  <si>
+    <t>50A87CBD7B7AFB1500998C4C99E2BAB11B410F90674CBEE37282958D7579C94C</t>
+  </si>
+  <si>
+    <t>93023A381E866DEAF0B7ADA3E3B11B42622EE9B28A20D65D5475D2AE03F771F3</t>
+  </si>
+  <si>
+    <t>A488B2E4EE7B4DA8B350CF29EE0ECE5249997DC65E4DD0542BC5892756B245A0</t>
   </si>
   <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
@@ -307,9 +319,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -326,6 +338,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
@@ -339,18 +358,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -371,9 +382,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -385,23 +426,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -409,21 +436,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -439,17 +460,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -461,16 +481,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -497,7 +509,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,73 +671,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,91 +689,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -766,17 +778,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -784,8 +790,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -801,32 +807,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -848,9 +828,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -859,155 +841,185 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3723,7 +3735,7 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -3846,8 +3858,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -3947,7 +3959,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -3967,7 +3979,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3976,7 +3988,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -4067,7 +4079,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -4076,7 +4088,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -4167,7 +4179,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -4176,7 +4188,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>

</xml_diff>

<commit_message>
Add Round 4 tasks
</commit_message>
<xml_diff>
--- a/hexp1989/evidence.xlsx
+++ b/hexp1989/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26700" windowHeight="13260" firstSheet="12" activeTab="21"/>
+    <workbookView windowWidth="26700" windowHeight="13260" firstSheet="15" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -32,13 +32,14 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="95">
   <si>
     <t>TeamName</t>
   </si>
@@ -307,10 +308,22 @@
     <t>A488B2E4EE7B4DA8B350CF29EE0ECE5249997DC65E4DD0542BC5892756B245A0</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
+    <t>6E43EE38CDC8C60B8244AB8DE9974B994DBCC2A963429BFF73E7D49C66B87C97</t>
+  </si>
+  <si>
+    <t>09870178A6B23F578398F5CF74DEACAA04631874E52D61ECEF332F35847672D9</t>
+  </si>
+  <si>
+    <t>641ED237750B8A32899CD049F3D1D3A1097E00E17382742077D626A003FFAD5B</t>
+  </si>
+  <si>
+    <t>DADB304570A358A8922B823FA818E7F387548EE1D2F6940BAA63A122C9021257</t>
+  </si>
+  <si>
+    <t>15D8E9EB1103EAE2CED5353BDFE3E809472288570C77C84C41596DE9DF3ABEF2</t>
+  </si>
+  <si>
+    <t>070590E72B7CD32A5207FAE60EF50D3C2E1D9320AA89F55877FD0E9E3609CB60</t>
   </si>
 </sst>
 </file>
@@ -318,10 +331,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -382,13 +395,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -403,8 +409,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -420,47 +450,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -474,15 +494,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -515,25 +528,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,19 +540,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,7 +564,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,19 +612,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,43 +684,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -659,37 +696,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -791,22 +804,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -828,6 +841,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -837,26 +859,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -878,142 +891,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1025,19 +1038,19 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2251,40 +2264,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="14.671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.8125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.171875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.171875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.421875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="43.8125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="43.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.171875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.171875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.671875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.421875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2322,77 +2335,77 @@
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="7"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:8">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:8">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:8">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:8">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:8">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:8">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2414,16 +2427,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="3"/>
@@ -2442,57 +2455,57 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -2517,16 +2530,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="3"/>
@@ -2545,57 +2558,57 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -2620,16 +2633,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="3"/>
@@ -2648,57 +2661,57 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -2723,16 +2736,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="3"/>
@@ -2751,57 +2764,57 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -2826,16 +2839,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3"/>
@@ -2854,10 +2867,10 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="4"/>
@@ -2865,10 +2878,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="4"/>
@@ -2876,10 +2889,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="4"/>
@@ -2887,36 +2900,36 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -2941,16 +2954,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3"/>
@@ -2969,10 +2982,10 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="4"/>
@@ -2980,10 +2993,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="4"/>
@@ -2991,10 +3004,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="4"/>
@@ -3002,36 +3015,36 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3056,16 +3069,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3"/>
@@ -3084,10 +3097,10 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C3" s="4"/>
@@ -3095,10 +3108,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="4"/>
@@ -3106,10 +3119,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="4"/>
@@ -3117,36 +3130,36 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3171,16 +3184,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3"/>
@@ -3199,10 +3212,10 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C3" s="4"/>
@@ -3210,10 +3223,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="4"/>
@@ -3221,10 +3234,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="4"/>
@@ -3232,36 +3245,36 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3286,16 +3299,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3"/>
@@ -3314,10 +3327,10 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="4"/>
@@ -3325,10 +3338,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="4"/>
@@ -3336,10 +3349,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="4"/>
@@ -3347,36 +3360,36 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3401,16 +3414,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3"/>
@@ -3429,10 +3442,10 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="4"/>
@@ -3440,10 +3453,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="4"/>
@@ -3451,10 +3464,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="4"/>
@@ -3462,36 +3475,36 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3516,15 +3529,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="2" width="17.8515625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="17.8515625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="3"/>
@@ -3543,57 +3556,57 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3618,16 +3631,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3"/>
@@ -3646,10 +3659,10 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="4"/>
@@ -3657,10 +3670,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="4"/>
@@ -3668,10 +3681,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="4"/>
@@ -3679,10 +3692,10 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="4"/>
@@ -3690,10 +3703,10 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="4"/>
@@ -3701,22 +3714,22 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3741,16 +3754,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3"/>
@@ -3769,10 +3782,10 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="4"/>
@@ -3780,10 +3793,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="4"/>
@@ -3791,10 +3804,10 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="4"/>
@@ -3802,10 +3815,10 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="4"/>
@@ -3813,10 +3826,10 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="4"/>
@@ -3824,22 +3837,22 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3858,18 +3871,18 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="3"/>
@@ -3887,7 +3900,7 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B3" s="4"/>
@@ -3896,49 +3909,49 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -3964,12 +3977,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="3"/>
@@ -3987,7 +4000,7 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="4"/>
@@ -3996,49 +4009,49 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4059,17 +4072,17 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="3"/>
@@ -4087,7 +4100,7 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" t="s">
         <v>90</v>
       </c>
       <c r="B3" s="4"/>
@@ -4096,49 +4109,49 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
+      <c r="A4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4158,18 +4171,18 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="3"/>
@@ -4179,7 +4192,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -4187,8 +4200,8 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
-        <v>90</v>
+      <c r="A3" t="s">
+        <v>92</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -4196,49 +4209,49 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -4250,6 +4263,38 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -4264,19 +4309,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="2" width="17.8515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="17.8515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.25" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="3"/>
@@ -4309,51 +4354,51 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
@@ -4377,24 +4422,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17.8515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6171875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.8515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.6171875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="3"/>
@@ -4403,7 +4448,7 @@
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -4415,59 +4460,59 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="4"/>
     </row>
   </sheetData>
@@ -4490,23 +4535,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="2" width="17.8515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="17.8515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="3"/>
@@ -4527,59 +4572,59 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="4"/>
     </row>
   </sheetData>
@@ -4602,23 +4647,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="2" width="17.8515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="17.8515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="3"/>
@@ -4639,59 +4684,59 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="4"/>
     </row>
   </sheetData>
@@ -4714,24 +4759,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17.8515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.8515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.3515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="3"/>
@@ -4752,59 +4797,59 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="4"/>
     </row>
   </sheetData>
@@ -4827,16 +4872,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="3"/>
@@ -4855,57 +4900,57 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -4930,16 +4975,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.8515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.8515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="3"/>
@@ -4958,57 +5003,57 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="13.55" customHeight="1" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>

</xml_diff>